<commit_message>
xlsParser doenst valiate missing param anymore
</commit_message>
<xml_diff>
--- a/test/libs/Xlsx/teste.xlsx
+++ b/test/libs/Xlsx/teste.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="141">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Especificação</t>
   </si>
   <si>
-    <t xml:space="preserve">Apresentação</t>
+    <t xml:space="preserve">'</t>
   </si>
   <si>
     <t xml:space="preserve">Moinhos Cruzeiro do Sul S.A.</t>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t xml:space="preserve">Panificação - Saco papel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sfd</t>
   </si>
   <si>
     <t xml:space="preserve">Farinha de Trigo pão congelado</t>
@@ -716,8 +719,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1376,6 +1379,11 @@
       </c>
       <c r="E38" s="2" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="1048240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1747,13 +1755,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>26</v>
@@ -1768,7 +1776,7 @@
         <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>26</v>
@@ -1783,7 +1791,7 @@
         <v>47</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>26</v>
@@ -1794,13 +1802,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>22</v>
@@ -1811,13 +1819,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>26</v>
@@ -1828,13 +1836,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>26</v>
@@ -1845,13 +1853,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>26</v>
@@ -1862,14 +1870,14 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>4</v>
@@ -1881,10 +1889,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>4</v>
@@ -1899,7 +1907,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>4</v>
@@ -1911,10 +1919,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>4</v>
@@ -1923,13 +1931,13 @@
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>4</v>
@@ -1938,13 +1946,13 @@
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>4</v>
@@ -1953,13 +1961,13 @@
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>4</v>
@@ -1967,7 +1975,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>10</v>
@@ -1976,7 +1984,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>4</v>
@@ -1988,10 +1996,10 @@
         <v>10</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>4</v>
@@ -2006,7 +2014,7 @@
         <v>34</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>4</v>
@@ -2015,13 +2023,13 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>4</v>
@@ -2030,13 +2038,13 @@
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>4</v>
@@ -2044,16 +2052,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>4</v>
@@ -2065,10 +2073,10 @@
         <v>10</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>4</v>
@@ -2080,10 +2088,10 @@
         <v>10</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>4</v>
@@ -2095,10 +2103,10 @@
         <v>10</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>4</v>
@@ -2110,10 +2118,10 @@
         <v>10</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>4</v>
@@ -2125,10 +2133,10 @@
         <v>10</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>4</v>
@@ -2140,10 +2148,10 @@
         <v>10</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>4</v>
@@ -2155,10 +2163,10 @@
         <v>10</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>4</v>
@@ -2170,10 +2178,10 @@
         <v>10</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>4</v>
@@ -2185,10 +2193,10 @@
         <v>10</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>4</v>
@@ -2196,16 +2204,16 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>4</v>
@@ -2213,16 +2221,16 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>4</v>
@@ -2231,13 +2239,13 @@
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9"/>
       <c r="B32" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C32" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>103</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>102</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>4</v>
@@ -2245,10 +2253,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>48</v>
@@ -2263,7 +2271,7 @@
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>34</v>
@@ -2278,10 +2286,10 @@
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
       <c r="B35" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>8</v>
@@ -2293,22 +2301,22 @@
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
       <c r="B37" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>48</v>
@@ -2323,7 +2331,7 @@
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3"/>
       <c r="B38" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>34</v>
@@ -2338,7 +2346,7 @@
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>48</v>
@@ -2356,7 +2364,7 @@
         <v>19</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>8</v>
@@ -2368,10 +2376,10 @@
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
       <c r="B41" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>8</v>
@@ -2383,10 +2391,10 @@
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>8</v>
@@ -2397,16 +2405,16 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>4</v>
@@ -2415,13 +2423,13 @@
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
       <c r="B44" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>4</v>
@@ -2430,13 +2438,13 @@
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>4</v>
@@ -2445,13 +2453,13 @@
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
       <c r="B46" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>4</v>
@@ -2459,13 +2467,13 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>22</v>
@@ -2476,13 +2484,13 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>16</v>
@@ -2493,16 +2501,16 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>4</v>
@@ -2514,10 +2522,10 @@
         <v>10</v>
       </c>
       <c r="C50" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>4</v>
@@ -2529,10 +2537,10 @@
         <v>10</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>4</v>
@@ -2544,10 +2552,10 @@
         <v>10</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>4</v>
@@ -2559,10 +2567,10 @@
         <v>10</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>4</v>
@@ -2574,10 +2582,10 @@
         <v>10</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>4</v>
@@ -2589,10 +2597,10 @@
         <v>10</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>4</v>
@@ -2604,10 +2612,10 @@
         <v>10</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>4</v>
@@ -2616,13 +2624,13 @@
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>4</v>
@@ -2631,13 +2639,13 @@
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
       <c r="B58" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>4</v>
@@ -2646,13 +2654,13 @@
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3"/>
       <c r="B59" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>4</v>
@@ -2661,13 +2669,13 @@
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>4</v>
@@ -2676,13 +2684,13 @@
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3"/>
       <c r="B61" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C61" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>133</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>4</v>
@@ -2691,13 +2699,13 @@
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3"/>
       <c r="B62" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>4</v>
@@ -2706,13 +2714,13 @@
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3"/>
       <c r="B63" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>4</v>
@@ -2721,13 +2729,13 @@
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3"/>
       <c r="B64" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>4</v>
@@ -2736,37 +2744,37 @@
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3"/>
       <c r="B65" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3"/>
       <c r="B66" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3"/>
       <c r="B67" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>